<commit_message>
still needs work but scrapes for links
</commit_message>
<xml_diff>
--- a/py-lending_tree/reviewlist.xlsx
+++ b/py-lending_tree/reviewlist.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,105 +434,75 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
+      <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/reliance-first-capital-llc/45102840</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/triumph-lending/44068646</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/silver-fin-capital-group/37405089</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/loansnap/39777117</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/planet-home-lending/57728064</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/grander-home-loans-inc/58426567</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/right-start-mortgage-inc/69298672</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/fairway-independent-mortgage-corporation/16236663</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/mortgage/new-american-funding/45679155</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>https://www.lendingtree.com/reviews/personal/upstart-network-inc/54350158</t>
         </is>

</xml_diff>